<commit_message>
Rerunning data paper analysis with latest iNat data and API preparing for bioblitz
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Ctenophora.xlsx
+++ b/data/dataPaper-I-in/arphified/Ctenophora.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10916" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11535" uniqueCount="572">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -1410,6 +1410,12 @@
     <t>Peter</t>
   </si>
   <si>
+    <t>Bolinopsis microptera</t>
+  </si>
+  <si>
+    <t>iNaturalist:1419827</t>
+  </si>
+  <si>
     <t>48.940296</t>
   </si>
   <si>
@@ -1587,6 +1593,18 @@
     <t>17:01:00</t>
   </si>
   <si>
+    <t>imerss.org:iNat:73721935</t>
+  </si>
+  <si>
+    <t>48.978121</t>
+  </si>
+  <si>
+    <t>-123.568355</t>
+  </si>
+  <si>
+    <t>08:42:00</t>
+  </si>
+  <si>
     <t>imerss.org:iNat:74472231</t>
   </si>
   <si>
@@ -1651,6 +1669,60 @@
   </si>
   <si>
     <t>19:11:00</t>
+  </si>
+  <si>
+    <t>imerss.org:iNat:92326440</t>
+  </si>
+  <si>
+    <t>48.901448</t>
+  </si>
+  <si>
+    <t>-123.445634</t>
+  </si>
+  <si>
+    <t>273</t>
+  </si>
+  <si>
+    <t>2021-05-07</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>imerss.org:iNat:100653654</t>
+  </si>
+  <si>
+    <t>48.871027</t>
+  </si>
+  <si>
+    <t>-123.313146</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>2021-11-06</t>
+  </si>
+  <si>
+    <t>14:18:00</t>
+  </si>
+  <si>
+    <t>imerss.org:iNat:116493737</t>
+  </si>
+  <si>
+    <t>Jackson W.F. Chu</t>
+  </si>
+  <si>
+    <t>48.912379</t>
+  </si>
+  <si>
+    <t>-123.327097</t>
+  </si>
+  <si>
+    <t>2008-05-24</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>Link type</t>
@@ -2564,7 +2636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EY70"/>
+  <dimension ref="A1:EY74"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -28308,7 +28380,7 @@
         <v>36</v>
       </c>
       <c r="S56" t="s">
-        <v>273</v>
+        <v>465</v>
       </c>
       <c r="T56" t="s">
         <v>36</v>
@@ -28323,7 +28395,7 @@
         <v>36</v>
       </c>
       <c r="X56" t="s">
-        <v>274</v>
+        <v>466</v>
       </c>
       <c r="Y56" t="s">
         <v>36</v>
@@ -28347,7 +28419,7 @@
         <v>36</v>
       </c>
       <c r="AF56" t="s">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="AG56" t="s">
         <v>36</v>
@@ -28383,22 +28455,22 @@
         <v>58</v>
       </c>
       <c r="AR56" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="AS56" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="AT56" t="s">
         <v>36</v>
       </c>
       <c r="AU56" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="AV56" t="s">
         <v>36</v>
       </c>
       <c r="AW56" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="AX56" t="s">
         <v>36</v>
@@ -28503,16 +28575,16 @@
         <v>36</v>
       </c>
       <c r="CF56" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="CG56" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="CH56" t="s">
         <v>36</v>
       </c>
       <c r="CI56" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="CJ56" t="s">
         <v>36</v>
@@ -28530,19 +28602,19 @@
         <v>36</v>
       </c>
       <c r="CO56" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="CP56" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="CQ56" t="s">
         <v>36</v>
       </c>
       <c r="CR56" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="CS56" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="CT56" t="s">
         <v>36</v>
@@ -28626,7 +28698,7 @@
         <v>36</v>
       </c>
       <c r="DU56" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="DV56" t="s">
         <v>36</v>
@@ -28692,7 +28764,7 @@
         <v>36</v>
       </c>
       <c r="EQ56" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER56" t="s">
         <v>36</v>
@@ -28724,7 +28796,7 @@
         <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C57" t="s">
         <v>36</v>
@@ -28739,7 +28811,7 @@
         <v>36</v>
       </c>
       <c r="G57" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="H57" t="s">
         <v>36</v>
@@ -28970,10 +29042,10 @@
         <v>36</v>
       </c>
       <c r="CF57" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="CG57" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="CH57" t="s">
         <v>36</v>
@@ -29093,10 +29165,10 @@
         <v>36</v>
       </c>
       <c r="DU57" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="DV57" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="DW57" t="s">
         <v>36</v>
@@ -29159,7 +29231,7 @@
         <v>36</v>
       </c>
       <c r="EQ57" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER57" t="s">
         <v>36</v>
@@ -29191,7 +29263,7 @@
         <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C58" t="s">
         <v>36</v>
@@ -29206,7 +29278,7 @@
         <v>36</v>
       </c>
       <c r="G58" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="H58" t="s">
         <v>36</v>
@@ -29242,7 +29314,7 @@
         <v>36</v>
       </c>
       <c r="S58" t="s">
-        <v>273</v>
+        <v>465</v>
       </c>
       <c r="T58" t="s">
         <v>36</v>
@@ -29257,7 +29329,7 @@
         <v>36</v>
       </c>
       <c r="X58" t="s">
-        <v>274</v>
+        <v>466</v>
       </c>
       <c r="Y58" t="s">
         <v>36</v>
@@ -29281,7 +29353,7 @@
         <v>36</v>
       </c>
       <c r="AF58" t="s">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="AG58" t="s">
         <v>36</v>
@@ -29317,22 +29389,22 @@
         <v>58</v>
       </c>
       <c r="AR58" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="AS58" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="AT58" t="s">
         <v>36</v>
       </c>
       <c r="AU58" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="AV58" t="s">
         <v>36</v>
       </c>
       <c r="AW58" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="AX58" t="s">
         <v>36</v>
@@ -29437,16 +29509,16 @@
         <v>36</v>
       </c>
       <c r="CF58" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="CG58" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="CH58" t="s">
         <v>36</v>
       </c>
       <c r="CI58" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="CJ58" t="s">
         <v>36</v>
@@ -29563,7 +29635,7 @@
         <v>456</v>
       </c>
       <c r="DV58" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="DW58" t="s">
         <v>36</v>
@@ -29626,7 +29698,7 @@
         <v>36</v>
       </c>
       <c r="EQ58" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER58" t="s">
         <v>36</v>
@@ -29658,7 +29730,7 @@
         <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C59" t="s">
         <v>36</v>
@@ -29673,7 +29745,7 @@
         <v>36</v>
       </c>
       <c r="G59" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H59" t="s">
         <v>36</v>
@@ -29904,10 +29976,10 @@
         <v>36</v>
       </c>
       <c r="CF59" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="CG59" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="CH59" t="s">
         <v>36</v>
@@ -29943,7 +30015,7 @@
         <v>36</v>
       </c>
       <c r="CS59" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="CT59" t="s">
         <v>36</v>
@@ -30027,10 +30099,10 @@
         <v>36</v>
       </c>
       <c r="DU59" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="DV59" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="DW59" t="s">
         <v>36</v>
@@ -30039,7 +30111,7 @@
         <v>36</v>
       </c>
       <c r="DY59" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="DZ59" t="s">
         <v>233</v>
@@ -30093,7 +30165,7 @@
         <v>36</v>
       </c>
       <c r="EQ59" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER59" t="s">
         <v>36</v>
@@ -30125,7 +30197,7 @@
         <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C60" t="s">
         <v>36</v>
@@ -30140,7 +30212,7 @@
         <v>36</v>
       </c>
       <c r="G60" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="H60" t="s">
         <v>36</v>
@@ -30371,10 +30443,10 @@
         <v>36</v>
       </c>
       <c r="CF60" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="CG60" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="CH60" t="s">
         <v>36</v>
@@ -30494,10 +30566,10 @@
         <v>36</v>
       </c>
       <c r="DU60" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="DV60" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="DW60" t="s">
         <v>36</v>
@@ -30506,7 +30578,7 @@
         <v>36</v>
       </c>
       <c r="DY60" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="DZ60" t="s">
         <v>233</v>
@@ -30560,7 +30632,7 @@
         <v>36</v>
       </c>
       <c r="EQ60" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER60" t="s">
         <v>36</v>
@@ -30592,7 +30664,7 @@
         <v>36</v>
       </c>
       <c r="B61" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C61" t="s">
         <v>36</v>
@@ -30838,10 +30910,10 @@
         <v>36</v>
       </c>
       <c r="CF61" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="CG61" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="CH61" t="s">
         <v>36</v>
@@ -30877,7 +30949,7 @@
         <v>36</v>
       </c>
       <c r="CS61" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="CT61" t="s">
         <v>36</v>
@@ -30961,10 +31033,10 @@
         <v>36</v>
       </c>
       <c r="DU61" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="DV61" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="DW61" t="s">
         <v>36</v>
@@ -30973,13 +31045,13 @@
         <v>36</v>
       </c>
       <c r="DY61" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ61" t="s">
         <v>262</v>
       </c>
       <c r="EA61" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="EB61" t="s">
         <v>36</v>
@@ -31027,7 +31099,7 @@
         <v>36</v>
       </c>
       <c r="EQ61" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER61" t="s">
         <v>36</v>
@@ -31059,7 +31131,7 @@
         <v>36</v>
       </c>
       <c r="B62" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C62" t="s">
         <v>36</v>
@@ -31074,7 +31146,7 @@
         <v>36</v>
       </c>
       <c r="G62" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="H62" t="s">
         <v>36</v>
@@ -31305,10 +31377,10 @@
         <v>36</v>
       </c>
       <c r="CF62" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="CG62" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="CH62" t="s">
         <v>36</v>
@@ -31428,7 +31500,7 @@
         <v>36</v>
       </c>
       <c r="DU62" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="DV62" t="s">
         <v>36</v>
@@ -31440,13 +31512,13 @@
         <v>36</v>
       </c>
       <c r="DY62" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ62" t="s">
         <v>262</v>
       </c>
       <c r="EA62" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="EB62" t="s">
         <v>36</v>
@@ -31494,7 +31566,7 @@
         <v>36</v>
       </c>
       <c r="EQ62" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER62" t="s">
         <v>36</v>
@@ -31526,7 +31598,7 @@
         <v>36</v>
       </c>
       <c r="B63" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C63" t="s">
         <v>36</v>
@@ -31541,7 +31613,7 @@
         <v>36</v>
       </c>
       <c r="G63" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H63" t="s">
         <v>36</v>
@@ -31772,10 +31844,10 @@
         <v>36</v>
       </c>
       <c r="CF63" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="CG63" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="CH63" t="s">
         <v>36</v>
@@ -31895,10 +31967,10 @@
         <v>36</v>
       </c>
       <c r="DU63" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="DV63" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="DW63" t="s">
         <v>36</v>
@@ -31907,7 +31979,7 @@
         <v>36</v>
       </c>
       <c r="DY63" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ63" t="s">
         <v>288</v>
@@ -31961,7 +32033,7 @@
         <v>36</v>
       </c>
       <c r="EQ63" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER63" t="s">
         <v>36</v>
@@ -31993,7 +32065,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C64" t="s">
         <v>36</v>
@@ -32008,7 +32080,7 @@
         <v>36</v>
       </c>
       <c r="G64" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H64" t="s">
         <v>36</v>
@@ -32239,10 +32311,10 @@
         <v>36</v>
       </c>
       <c r="CF64" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="CG64" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="CH64" t="s">
         <v>36</v>
@@ -32362,10 +32434,10 @@
         <v>36</v>
       </c>
       <c r="DU64" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="DV64" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="DW64" t="s">
         <v>36</v>
@@ -32374,7 +32446,7 @@
         <v>36</v>
       </c>
       <c r="DY64" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ64" t="s">
         <v>288</v>
@@ -32428,7 +32500,7 @@
         <v>36</v>
       </c>
       <c r="EQ64" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER64" t="s">
         <v>36</v>
@@ -32460,7 +32532,7 @@
         <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
@@ -32475,7 +32547,7 @@
         <v>36</v>
       </c>
       <c r="G65" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H65" t="s">
         <v>36</v>
@@ -32706,16 +32778,16 @@
         <v>36</v>
       </c>
       <c r="CF65" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="CG65" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="CH65" t="s">
         <v>36</v>
       </c>
       <c r="CI65" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="CJ65" t="s">
         <v>36</v>
@@ -32829,10 +32901,10 @@
         <v>36</v>
       </c>
       <c r="DU65" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="DV65" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="DW65" t="s">
         <v>36</v>
@@ -32841,7 +32913,7 @@
         <v>36</v>
       </c>
       <c r="DY65" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ65" t="s">
         <v>288</v>
@@ -32895,7 +32967,7 @@
         <v>36</v>
       </c>
       <c r="EQ65" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER65" t="s">
         <v>36</v>
@@ -32927,7 +32999,7 @@
         <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C66" t="s">
         <v>36</v>
@@ -32942,7 +33014,7 @@
         <v>36</v>
       </c>
       <c r="G66" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H66" t="s">
         <v>36</v>
@@ -32978,7 +33050,7 @@
         <v>36</v>
       </c>
       <c r="S66" t="s">
-        <v>273</v>
+        <v>465</v>
       </c>
       <c r="T66" t="s">
         <v>36</v>
@@ -32993,7 +33065,7 @@
         <v>36</v>
       </c>
       <c r="X66" t="s">
-        <v>274</v>
+        <v>466</v>
       </c>
       <c r="Y66" t="s">
         <v>36</v>
@@ -33017,7 +33089,7 @@
         <v>36</v>
       </c>
       <c r="AF66" t="s">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="AG66" t="s">
         <v>36</v>
@@ -33053,22 +33125,22 @@
         <v>58</v>
       </c>
       <c r="AR66" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="AS66" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="AT66" t="s">
         <v>36</v>
       </c>
       <c r="AU66" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="AV66" t="s">
         <v>36</v>
       </c>
       <c r="AW66" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="AX66" t="s">
         <v>36</v>
@@ -33173,16 +33245,16 @@
         <v>36</v>
       </c>
       <c r="CF66" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="CG66" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="CH66" t="s">
         <v>36</v>
       </c>
       <c r="CI66" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="CJ66" t="s">
         <v>36</v>
@@ -33296,10 +33368,10 @@
         <v>36</v>
       </c>
       <c r="DU66" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="DV66" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="DW66" t="s">
         <v>36</v>
@@ -33308,7 +33380,7 @@
         <v>36</v>
       </c>
       <c r="DY66" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ66" t="s">
         <v>288</v>
@@ -33362,7 +33434,7 @@
         <v>36</v>
       </c>
       <c r="EQ66" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER66" t="s">
         <v>36</v>
@@ -33394,7 +33466,7 @@
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C67" t="s">
         <v>36</v>
@@ -33409,7 +33481,7 @@
         <v>36</v>
       </c>
       <c r="G67" t="s">
-        <v>468</v>
+        <v>509</v>
       </c>
       <c r="H67" t="s">
         <v>36</v>
@@ -33640,16 +33712,16 @@
         <v>36</v>
       </c>
       <c r="CF67" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="CG67" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="CH67" t="s">
         <v>36</v>
       </c>
       <c r="CI67" t="s">
-        <v>527</v>
+        <v>288</v>
       </c>
       <c r="CJ67" t="s">
         <v>36</v>
@@ -33763,7 +33835,7 @@
         <v>36</v>
       </c>
       <c r="DU67" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="DV67" t="s">
         <v>529</v>
@@ -33775,13 +33847,13 @@
         <v>36</v>
       </c>
       <c r="DY67" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ67" t="s">
         <v>288</v>
       </c>
       <c r="EA67" t="s">
-        <v>530</v>
+        <v>368</v>
       </c>
       <c r="EB67" t="s">
         <v>36</v>
@@ -33829,7 +33901,7 @@
         <v>36</v>
       </c>
       <c r="EQ67" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER67" t="s">
         <v>36</v>
@@ -33861,7 +33933,7 @@
         <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C68" t="s">
         <v>36</v>
@@ -33876,7 +33948,7 @@
         <v>36</v>
       </c>
       <c r="G68" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H68" t="s">
         <v>36</v>
@@ -33912,7 +33984,7 @@
         <v>36</v>
       </c>
       <c r="S68" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="T68" t="s">
         <v>36</v>
@@ -33927,7 +33999,7 @@
         <v>36</v>
       </c>
       <c r="X68" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="Y68" t="s">
         <v>36</v>
@@ -33951,7 +34023,7 @@
         <v>36</v>
       </c>
       <c r="AF68" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="AG68" t="s">
         <v>36</v>
@@ -33978,19 +34050,19 @@
         <v>37</v>
       </c>
       <c r="AO68" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AP68" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AQ68" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="AR68" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="AS68" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="AT68" t="s">
         <v>36</v>
@@ -34002,7 +34074,7 @@
         <v>36</v>
       </c>
       <c r="AW68" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AX68" t="s">
         <v>36</v>
@@ -34107,17 +34179,17 @@
         <v>36</v>
       </c>
       <c r="CF68" t="s">
+        <v>531</v>
+      </c>
+      <c r="CG68" t="s">
         <v>532</v>
       </c>
-      <c r="CG68" t="s">
+      <c r="CH68" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI68" t="s">
         <v>533</v>
       </c>
-      <c r="CH68" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI68" t="s">
-        <v>234</v>
-      </c>
       <c r="CJ68" t="s">
         <v>36</v>
       </c>
@@ -34230,10 +34302,10 @@
         <v>36</v>
       </c>
       <c r="DU68" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="DV68" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="DW68" t="s">
         <v>36</v>
@@ -34242,13 +34314,13 @@
         <v>36</v>
       </c>
       <c r="DY68" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ68" t="s">
         <v>288</v>
       </c>
       <c r="EA68" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="EB68" t="s">
         <v>36</v>
@@ -34296,7 +34368,7 @@
         <v>36</v>
       </c>
       <c r="EQ68" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER68" t="s">
         <v>36</v>
@@ -34328,7 +34400,7 @@
         <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C69" t="s">
         <v>36</v>
@@ -34343,7 +34415,7 @@
         <v>36</v>
       </c>
       <c r="G69" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H69" t="s">
         <v>36</v>
@@ -34379,7 +34451,7 @@
         <v>36</v>
       </c>
       <c r="S69" t="s">
-        <v>273</v>
+        <v>220</v>
       </c>
       <c r="T69" t="s">
         <v>36</v>
@@ -34394,7 +34466,7 @@
         <v>36</v>
       </c>
       <c r="X69" t="s">
-        <v>274</v>
+        <v>221</v>
       </c>
       <c r="Y69" t="s">
         <v>36</v>
@@ -34418,7 +34490,7 @@
         <v>36</v>
       </c>
       <c r="AF69" t="s">
-        <v>273</v>
+        <v>220</v>
       </c>
       <c r="AG69" t="s">
         <v>36</v>
@@ -34448,16 +34520,16 @@
         <v>45</v>
       </c>
       <c r="AP69" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="AQ69" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="AR69" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="AS69" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AT69" t="s">
         <v>36</v>
@@ -34469,7 +34541,7 @@
         <v>36</v>
       </c>
       <c r="AW69" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="AX69" t="s">
         <v>36</v>
@@ -34574,16 +34646,16 @@
         <v>36</v>
       </c>
       <c r="CF69" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="CG69" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="CH69" t="s">
         <v>36</v>
       </c>
       <c r="CI69" t="s">
-        <v>538</v>
+        <v>234</v>
       </c>
       <c r="CJ69" t="s">
         <v>36</v>
@@ -34697,10 +34769,10 @@
         <v>36</v>
       </c>
       <c r="DU69" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="DV69" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="DW69" t="s">
         <v>36</v>
@@ -34709,13 +34781,13 @@
         <v>36</v>
       </c>
       <c r="DY69" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ69" t="s">
         <v>288</v>
       </c>
       <c r="EA69" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="EB69" t="s">
         <v>36</v>
@@ -34763,7 +34835,7 @@
         <v>36</v>
       </c>
       <c r="EQ69" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER69" t="s">
         <v>36</v>
@@ -34795,7 +34867,7 @@
         <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C70" t="s">
         <v>36</v>
@@ -34810,7 +34882,7 @@
         <v>36</v>
       </c>
       <c r="G70" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H70" t="s">
         <v>36</v>
@@ -34846,7 +34918,7 @@
         <v>36</v>
       </c>
       <c r="S70" t="s">
-        <v>220</v>
+        <v>465</v>
       </c>
       <c r="T70" t="s">
         <v>36</v>
@@ -34861,7 +34933,7 @@
         <v>36</v>
       </c>
       <c r="X70" t="s">
-        <v>221</v>
+        <v>466</v>
       </c>
       <c r="Y70" t="s">
         <v>36</v>
@@ -34885,7 +34957,7 @@
         <v>36</v>
       </c>
       <c r="AF70" t="s">
-        <v>220</v>
+        <v>36</v>
       </c>
       <c r="AG70" t="s">
         <v>36</v>
@@ -34915,28 +34987,28 @@
         <v>45</v>
       </c>
       <c r="AP70" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="AQ70" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AR70" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="AS70" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="AT70" t="s">
         <v>36</v>
       </c>
       <c r="AU70" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="AV70" t="s">
         <v>36</v>
       </c>
       <c r="AW70" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="AX70" t="s">
         <v>36</v>
@@ -35041,16 +35113,16 @@
         <v>36</v>
       </c>
       <c r="CF70" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="CG70" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="CH70" t="s">
         <v>36</v>
       </c>
       <c r="CI70" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="CJ70" t="s">
         <v>36</v>
@@ -35164,7 +35236,7 @@
         <v>36</v>
       </c>
       <c r="DU70" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="DV70" t="s">
         <v>545</v>
@@ -35176,13 +35248,13 @@
         <v>36</v>
       </c>
       <c r="DY70" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="DZ70" t="s">
         <v>288</v>
       </c>
       <c r="EA70" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="EB70" t="s">
         <v>36</v>
@@ -35230,7 +35302,7 @@
         <v>36</v>
       </c>
       <c r="EQ70" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="ER70" t="s">
         <v>36</v>
@@ -35254,6 +35326,1874 @@
         <v>36</v>
       </c>
       <c r="EY70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" t="s">
+        <v>546</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G71" t="s">
+        <v>470</v>
+      </c>
+      <c r="H71" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" t="s">
+        <v>36</v>
+      </c>
+      <c r="J71" t="s">
+        <v>36</v>
+      </c>
+      <c r="K71" t="s">
+        <v>36</v>
+      </c>
+      <c r="L71" t="s">
+        <v>36</v>
+      </c>
+      <c r="M71" t="s">
+        <v>36</v>
+      </c>
+      <c r="N71" t="s">
+        <v>36</v>
+      </c>
+      <c r="O71" t="s">
+        <v>219</v>
+      </c>
+      <c r="P71" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>36</v>
+      </c>
+      <c r="R71" t="s">
+        <v>36</v>
+      </c>
+      <c r="S71" t="s">
+        <v>220</v>
+      </c>
+      <c r="T71" t="s">
+        <v>36</v>
+      </c>
+      <c r="U71" t="s">
+        <v>36</v>
+      </c>
+      <c r="V71" t="s">
+        <v>36</v>
+      </c>
+      <c r="W71" t="s">
+        <v>36</v>
+      </c>
+      <c r="X71" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM71" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN71" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO71" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ71" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR71" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS71" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU71" t="s">
+        <v>222</v>
+      </c>
+      <c r="AV71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW71" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY71" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI71" t="s">
+        <v>223</v>
+      </c>
+      <c r="BJ71" t="s">
+        <v>224</v>
+      </c>
+      <c r="BK71" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL71" t="s">
+        <v>226</v>
+      </c>
+      <c r="BM71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY71" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF71" t="s">
+        <v>547</v>
+      </c>
+      <c r="CG71" t="s">
+        <v>548</v>
+      </c>
+      <c r="CH71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI71" t="s">
+        <v>549</v>
+      </c>
+      <c r="CJ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY71" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU71" t="s">
+        <v>550</v>
+      </c>
+      <c r="DV71" t="s">
+        <v>551</v>
+      </c>
+      <c r="DW71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX71" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY71" t="s">
+        <v>506</v>
+      </c>
+      <c r="DZ71" t="s">
+        <v>288</v>
+      </c>
+      <c r="EA71" t="s">
+        <v>507</v>
+      </c>
+      <c r="EB71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC71" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EF71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EG71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ71" t="s">
+        <v>475</v>
+      </c>
+      <c r="ER71" t="s">
+        <v>36</v>
+      </c>
+      <c r="ES71" t="s">
+        <v>36</v>
+      </c>
+      <c r="ET71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU71" t="s">
+        <v>237</v>
+      </c>
+      <c r="EV71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EW71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EX71" t="s">
+        <v>36</v>
+      </c>
+      <c r="EY71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" t="s">
+        <v>552</v>
+      </c>
+      <c r="C72" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" t="s">
+        <v>36</v>
+      </c>
+      <c r="E72" t="s">
+        <v>36</v>
+      </c>
+      <c r="F72" t="s">
+        <v>36</v>
+      </c>
+      <c r="G72" t="s">
+        <v>496</v>
+      </c>
+      <c r="H72" t="s">
+        <v>36</v>
+      </c>
+      <c r="I72" t="s">
+        <v>36</v>
+      </c>
+      <c r="J72" t="s">
+        <v>36</v>
+      </c>
+      <c r="K72" t="s">
+        <v>36</v>
+      </c>
+      <c r="L72" t="s">
+        <v>36</v>
+      </c>
+      <c r="M72" t="s">
+        <v>36</v>
+      </c>
+      <c r="N72" t="s">
+        <v>36</v>
+      </c>
+      <c r="O72" t="s">
+        <v>219</v>
+      </c>
+      <c r="P72" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>36</v>
+      </c>
+      <c r="R72" t="s">
+        <v>36</v>
+      </c>
+      <c r="S72" t="s">
+        <v>220</v>
+      </c>
+      <c r="T72" t="s">
+        <v>36</v>
+      </c>
+      <c r="U72" t="s">
+        <v>36</v>
+      </c>
+      <c r="V72" t="s">
+        <v>36</v>
+      </c>
+      <c r="W72" t="s">
+        <v>36</v>
+      </c>
+      <c r="X72" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF72" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM72" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN72" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO72" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP72" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ72" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR72" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS72" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU72" t="s">
+        <v>222</v>
+      </c>
+      <c r="AV72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW72" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY72" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI72" t="s">
+        <v>223</v>
+      </c>
+      <c r="BJ72" t="s">
+        <v>224</v>
+      </c>
+      <c r="BK72" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL72" t="s">
+        <v>226</v>
+      </c>
+      <c r="BM72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY72" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF72" t="s">
+        <v>553</v>
+      </c>
+      <c r="CG72" t="s">
+        <v>554</v>
+      </c>
+      <c r="CH72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI72" t="s">
+        <v>555</v>
+      </c>
+      <c r="CJ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY72" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU72" t="s">
+        <v>556</v>
+      </c>
+      <c r="DV72" t="s">
+        <v>557</v>
+      </c>
+      <c r="DW72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX72" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY72" t="s">
+        <v>506</v>
+      </c>
+      <c r="DZ72" t="s">
+        <v>233</v>
+      </c>
+      <c r="EA72" t="s">
+        <v>245</v>
+      </c>
+      <c r="EB72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC72" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EF72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EG72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ72" t="s">
+        <v>475</v>
+      </c>
+      <c r="ER72" t="s">
+        <v>36</v>
+      </c>
+      <c r="ES72" t="s">
+        <v>36</v>
+      </c>
+      <c r="ET72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU72" t="s">
+        <v>237</v>
+      </c>
+      <c r="EV72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EW72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EX72" t="s">
+        <v>36</v>
+      </c>
+      <c r="EY72" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" t="s">
+        <v>558</v>
+      </c>
+      <c r="C73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" t="s">
+        <v>36</v>
+      </c>
+      <c r="F73" t="s">
+        <v>36</v>
+      </c>
+      <c r="G73" t="s">
+        <v>470</v>
+      </c>
+      <c r="H73" t="s">
+        <v>36</v>
+      </c>
+      <c r="I73" t="s">
+        <v>36</v>
+      </c>
+      <c r="J73" t="s">
+        <v>36</v>
+      </c>
+      <c r="K73" t="s">
+        <v>36</v>
+      </c>
+      <c r="L73" t="s">
+        <v>36</v>
+      </c>
+      <c r="M73" t="s">
+        <v>36</v>
+      </c>
+      <c r="N73" t="s">
+        <v>36</v>
+      </c>
+      <c r="O73" t="s">
+        <v>219</v>
+      </c>
+      <c r="P73" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>36</v>
+      </c>
+      <c r="R73" t="s">
+        <v>36</v>
+      </c>
+      <c r="S73" t="s">
+        <v>465</v>
+      </c>
+      <c r="T73" t="s">
+        <v>36</v>
+      </c>
+      <c r="U73" t="s">
+        <v>36</v>
+      </c>
+      <c r="V73" t="s">
+        <v>36</v>
+      </c>
+      <c r="W73" t="s">
+        <v>36</v>
+      </c>
+      <c r="X73" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM73" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN73" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO73" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ73" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU73" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY73" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI73" t="s">
+        <v>223</v>
+      </c>
+      <c r="BJ73" t="s">
+        <v>224</v>
+      </c>
+      <c r="BK73" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL73" t="s">
+        <v>226</v>
+      </c>
+      <c r="BM73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY73" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF73" t="s">
+        <v>559</v>
+      </c>
+      <c r="CG73" t="s">
+        <v>560</v>
+      </c>
+      <c r="CH73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI73" t="s">
+        <v>561</v>
+      </c>
+      <c r="CJ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY73" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU73" t="s">
+        <v>562</v>
+      </c>
+      <c r="DV73" t="s">
+        <v>563</v>
+      </c>
+      <c r="DW73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX73" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY73" t="s">
+        <v>506</v>
+      </c>
+      <c r="DZ73" t="s">
+        <v>368</v>
+      </c>
+      <c r="EA73" t="s">
+        <v>327</v>
+      </c>
+      <c r="EB73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC73" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EF73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EG73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ73" t="s">
+        <v>475</v>
+      </c>
+      <c r="ER73" t="s">
+        <v>36</v>
+      </c>
+      <c r="ES73" t="s">
+        <v>36</v>
+      </c>
+      <c r="ET73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU73" t="s">
+        <v>237</v>
+      </c>
+      <c r="EV73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EW73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EX73" t="s">
+        <v>36</v>
+      </c>
+      <c r="EY73" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" t="s">
+        <v>564</v>
+      </c>
+      <c r="C74" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" t="s">
+        <v>565</v>
+      </c>
+      <c r="H74" t="s">
+        <v>36</v>
+      </c>
+      <c r="I74" t="s">
+        <v>36</v>
+      </c>
+      <c r="J74" t="s">
+        <v>36</v>
+      </c>
+      <c r="K74" t="s">
+        <v>36</v>
+      </c>
+      <c r="L74" t="s">
+        <v>36</v>
+      </c>
+      <c r="M74" t="s">
+        <v>36</v>
+      </c>
+      <c r="N74" t="s">
+        <v>36</v>
+      </c>
+      <c r="O74" t="s">
+        <v>219</v>
+      </c>
+      <c r="P74" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>36</v>
+      </c>
+      <c r="R74" t="s">
+        <v>36</v>
+      </c>
+      <c r="S74" t="s">
+        <v>465</v>
+      </c>
+      <c r="T74" t="s">
+        <v>36</v>
+      </c>
+      <c r="U74" t="s">
+        <v>36</v>
+      </c>
+      <c r="V74" t="s">
+        <v>36</v>
+      </c>
+      <c r="W74" t="s">
+        <v>36</v>
+      </c>
+      <c r="X74" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM74" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN74" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO74" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ74" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU74" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY74" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI74" t="s">
+        <v>223</v>
+      </c>
+      <c r="BJ74" t="s">
+        <v>224</v>
+      </c>
+      <c r="BK74" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL74" t="s">
+        <v>226</v>
+      </c>
+      <c r="BM74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY74" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF74" t="s">
+        <v>566</v>
+      </c>
+      <c r="CG74" t="s">
+        <v>567</v>
+      </c>
+      <c r="CH74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI74">
+        <v>100</v>
+      </c>
+      <c r="CJ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS74" t="s">
+        <v>491</v>
+      </c>
+      <c r="CT74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY74" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU74" t="s">
+        <v>568</v>
+      </c>
+      <c r="DV74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DW74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX74" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY74" t="s">
+        <v>310</v>
+      </c>
+      <c r="DZ74" t="s">
+        <v>233</v>
+      </c>
+      <c r="EA74" t="s">
+        <v>569</v>
+      </c>
+      <c r="EB74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC74" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EF74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EG74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ74" t="s">
+        <v>475</v>
+      </c>
+      <c r="ER74" t="s">
+        <v>36</v>
+      </c>
+      <c r="ES74" t="s">
+        <v>36</v>
+      </c>
+      <c r="ET74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU74" t="s">
+        <v>237</v>
+      </c>
+      <c r="EV74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EW74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EX74" t="s">
+        <v>36</v>
+      </c>
+      <c r="EY74" t="s">
         <v>36</v>
       </c>
     </row>
@@ -35273,10 +37213,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>546</v>
+        <v>570</v>
       </c>
       <c r="C1" t="s">
-        <v>547</v>
+        <v>571</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>